<commit_message>
Post Subscription Template Modification
</commit_message>
<xml_diff>
--- a/tmpp-core/src/main/resources/execute_plan_template.xlsx
+++ b/tmpp-core/src/main/resources/execute_plan_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE155ED-0A13-4C7D-83E3-0FE4BFAB2CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D12237-AFD5-44B6-BA93-82DCD7B626BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>开课年级</t>
+    <t>年级</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -138,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -166,8 +166,36 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -177,7 +205,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,7 +231,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -507,7 +538,7 @@
     <col min="10" max="10" width="32" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -519,57 +550,55 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -581,7 +610,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -593,7 +622,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -605,7 +634,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -617,7 +646,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -629,7 +658,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -641,7 +670,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -653,7 +682,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -665,7 +694,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -677,7 +706,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -689,7 +718,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -701,7 +730,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -713,7 +742,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -871,14 +900,14 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{5F3554B6-CA3B-4C7E-91A6-718F5CF90437}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F1048576" xr:uid="{5F3554B6-CA3B-4C7E-91A6-718F5CF90437}">
       <formula1>"考试,考察"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{38EAA81E-4C63-4A76-851E-6F13AEC460B6}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H1048576" xr:uid="{38EAA81E-4C63-4A76-851E-6F13AEC460B6}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>